<commit_message>
Add financial data integration, tracing, and sidebar cleanup
- Integrated financial data from vte_financial_data.xlsx with Patient_Costs sheet
- Added new Financial Analytics page with patient costs, department budgets, ROI summary, and platform costs
- Added Application Insights tracing service for Azure AI Foundry monitoring
- Removed Cost Summary from sidebar (moved to Cost Tracking page)
- Updated chat interface with tracing and financial-aware suggested questions
- Added error handling for Excel file permission issues
- Archived current working scripts to archive/ folder
- Removed hardcoded API keys from tracing script
</commit_message>
<xml_diff>
--- a/data/vte_sample_data.xlsx
+++ b/data/vte_sample_data.xlsx
@@ -11322,4 +11322,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{87ba5c36-b7cf-4793-bbc2-bd5b3a9f95ca}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>